<commit_message>
Actualización de las horas de las evidencias
</commit_message>
<xml_diff>
--- a/Evidencias/Evidencias Grupo 2.xlsx
+++ b/Evidencias/Evidencias Grupo 2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\Desktop\Comunicación\Comunicacion\Evidencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Juan</t>
   </si>
   <si>
-    <t>21 horas y 40 minutos</t>
-  </si>
-  <si>
     <t>Secretario y web</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>Excel realizado durante las jornadas</t>
+  </si>
+  <si>
+    <t>22 horas y 20 minutos</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
   <dimension ref="A1:Y9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,25 +705,25 @@
         <v>11</v>
       </c>
       <c r="S1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>2</v>
@@ -763,16 +763,16 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>2</v>
@@ -805,25 +805,25 @@
         <v>11</v>
       </c>
       <c r="S3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="X3" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="Y3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -834,16 +834,16 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>2</v>
@@ -875,16 +875,16 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>2</v>
@@ -916,16 +916,16 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>2</v>
@@ -954,16 +954,16 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>2</v>
@@ -1004,16 +1004,16 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>44</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>2</v>
@@ -1054,16 +1054,16 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>2</v>

</xml_diff>